<commit_message>
updated the code with Silver NanoParticles
</commit_message>
<xml_diff>
--- a/data/Toxicity Measurements -- Meta Analysis.xlsx
+++ b/data/Toxicity Measurements -- Meta Analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="paper_summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,33 +15,6 @@
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="F1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Aahana, why this column?
-	-Suren Kumar
-+aahanang@gmail.com : Your attention is needed
-	-Suren Kumar</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -146,7 +119,7 @@
   </si>
   <si>
     <t>- Male
-- Weight </t>
+- Weight</t>
   </si>
   <si>
     <t>- Diameter (nm)
@@ -369,7 +342,7 @@
     <t>BAL Macrophages Control</t>
   </si>
   <si>
-    <t>BAL Macrophages </t>
+    <t>BAL Macrophages</t>
   </si>
   <si>
     <t>BAL Macrophages SD</t>
@@ -387,7 +360,7 @@
     <t>BAL LDH Control</t>
   </si>
   <si>
-    <t>BAL LDH </t>
+    <t>BAL LDH</t>
   </si>
   <si>
     <t>BAL LDH SD</t>
@@ -396,7 +369,7 @@
     <t>BAL Total Protein Control</t>
   </si>
   <si>
-    <t>BAL Total Protein </t>
+    <t>BAL Total Protein</t>
   </si>
   <si>
     <t>BAL Total Protein SD</t>
@@ -747,10 +720,10 @@
   </sheetPr>
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="Q25" activeCellId="0" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1601,6 +1574,9 @@
       <c r="O10" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q10" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R10" s="2" t="n">
         <v>1</v>
       </c>
@@ -1671,6 +1647,9 @@
       <c r="O11" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q11" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R11" s="2" t="n">
         <v>1</v>
       </c>
@@ -1741,6 +1720,9 @@
       <c r="O12" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q12" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R12" s="2" t="n">
         <v>7</v>
       </c>
@@ -1811,6 +1793,9 @@
       <c r="O13" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q13" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R13" s="2" t="n">
         <v>7</v>
       </c>
@@ -1881,6 +1866,9 @@
       <c r="O14" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q14" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R14" s="2" t="n">
         <v>21</v>
       </c>
@@ -1951,6 +1939,9 @@
       <c r="O15" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q15" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R15" s="2" t="n">
         <v>21</v>
       </c>
@@ -2021,6 +2012,9 @@
       <c r="O16" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q16" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R16" s="2" t="n">
         <v>1</v>
       </c>
@@ -2091,6 +2085,9 @@
       <c r="O17" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q17" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R17" s="2" t="n">
         <v>1</v>
       </c>
@@ -2161,6 +2158,9 @@
       <c r="O18" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R18" s="2" t="n">
         <v>1</v>
       </c>
@@ -2231,6 +2231,9 @@
       <c r="O19" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q19" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R19" s="2" t="n">
         <v>1</v>
       </c>
@@ -2301,6 +2304,9 @@
       <c r="O20" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q20" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R20" s="2" t="n">
         <v>7</v>
       </c>
@@ -2371,6 +2377,9 @@
       <c r="O21" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q21" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R21" s="2" t="n">
         <v>7</v>
       </c>
@@ -2441,6 +2450,9 @@
       <c r="O22" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q22" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R22" s="2" t="n">
         <v>7</v>
       </c>
@@ -2511,6 +2523,9 @@
       <c r="O23" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q23" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R23" s="2" t="n">
         <v>7</v>
       </c>
@@ -2581,6 +2596,9 @@
       <c r="O24" s="2" t="n">
         <v>100</v>
       </c>
+      <c r="Q24" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="R24" s="2" t="n">
         <v>21</v>
       </c>
@@ -2650,6 +2668,9 @@
       </c>
       <c r="O25" s="2" t="n">
         <v>100</v>
+      </c>
+      <c r="Q25" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="R25" s="2" t="n">
         <v>21</v>
@@ -3067,7 +3088,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5308,7 +5328,7 @@
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>